<commit_message>
overflow logic reverted for better accuracy, new file creation logic added (removed overwrite)
</commit_message>
<xml_diff>
--- a/admission_cutoffs_output.xlsx
+++ b/admission_cutoffs_output.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K229"/>
+  <dimension ref="A1:K227"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9348,88 +9348,6 @@
       <c r="J227" t="inlineStr"/>
       <c r="K227" t="inlineStr"/>
     </row>
-    <row r="228">
-      <c r="A228" t="inlineStr"/>
-      <c r="B228" t="inlineStr"/>
-      <c r="C228" t="inlineStr"/>
-      <c r="D228" t="inlineStr">
-        <is>
-          <t>0110524610</t>
-        </is>
-      </c>
-      <c r="E228" t="inlineStr">
-        <is>
-          <t>Information Technology</t>
-        </is>
-      </c>
-      <c r="F228" t="inlineStr">
-        <is>
-          <t>Un-Aided Autonomous</t>
-        </is>
-      </c>
-      <c r="G228" t="inlineStr">
-        <is>
-          <t>State Level</t>
-        </is>
-      </c>
-      <c r="H228" t="inlineStr">
-        <is>
-          <t>VII</t>
-        </is>
-      </c>
-      <c r="I228" t="inlineStr">
-        <is>
-          <t>TFWS</t>
-        </is>
-      </c>
-      <c r="J228" t="inlineStr"/>
-      <c r="K228" t="inlineStr"/>
-    </row>
-    <row r="229">
-      <c r="A229" t="inlineStr"/>
-      <c r="B229" t="inlineStr"/>
-      <c r="C229" t="inlineStr"/>
-      <c r="D229" t="inlineStr">
-        <is>
-          <t>0110524610</t>
-        </is>
-      </c>
-      <c r="E229" t="inlineStr">
-        <is>
-          <t>Information Technology</t>
-        </is>
-      </c>
-      <c r="F229" t="inlineStr">
-        <is>
-          <t>Un-Aided Autonomous</t>
-        </is>
-      </c>
-      <c r="G229" t="inlineStr">
-        <is>
-          <t>State Level</t>
-        </is>
-      </c>
-      <c r="H229" t="inlineStr">
-        <is>
-          <t>VII</t>
-        </is>
-      </c>
-      <c r="I229" t="inlineStr">
-        <is>
-          <t>ORPHAN</t>
-        </is>
-      </c>
-      <c r="J229" t="inlineStr">
-        <is>
-          <t>87619</t>
-        </is>
-      </c>
-      <c r="K229" t="inlineStr">
-        <is>
-          <t>67.6869909</t>
-        </is>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>